<commit_message>
Updated Vaishakhi Pilankar Diary
</commit_message>
<xml_diff>
--- a/diaries/diary-vaishakhi-pilankar.xlsx
+++ b/diaries/diary-vaishakhi-pilankar.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guds\Desktop\MSWE\CourseWork\Winter 2020\265P\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guds\Desktop\MSWE\CourseWork\Winter_2020\265P\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB57919-00CB-457B-9173-A580AAB34A5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01BDA6D-95BA-47F5-BB5B-5878AF1968C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-108" windowWidth="22308" windowHeight="13176" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -75,9 +75,6 @@
     <t>vaishakhiification</t>
   </si>
   <si>
-    <t>05:00 pm - 07:00 pm</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -91,6 +88,84 @@
   </si>
   <si>
     <t>Excited to see what this course has to offer.</t>
+  </si>
+  <si>
+    <t>11:00 am - 02:00 pm</t>
+  </si>
+  <si>
+    <t>To successfully build and run 3 projects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Was able to run 2 projects. </t>
+  </si>
+  <si>
+    <t>Had some trouble building the projects. Maybe I should've read the readme thoroughly first.</t>
+  </si>
+  <si>
+    <t>Little frustated about fixing the errors. Errors were a little random.</t>
+  </si>
+  <si>
+    <t>Team formation</t>
+  </si>
+  <si>
+    <t>Formed a group of three members for the project and added the team information on Excel sheet</t>
+  </si>
+  <si>
+    <t>Anjana, Aman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need to learn git properly. </t>
+  </si>
+  <si>
+    <t>Excited to be working with my team for the rest of the quarter</t>
+  </si>
+  <si>
+    <t>05:00 pm - 07:50 pm</t>
+  </si>
+  <si>
+    <t>Didn't know what to expect. Probably learn more about code reading and understanding.</t>
+  </si>
+  <si>
+    <t>Was able to check the code to understand its functionality briefly by successfully navigating through the project. Felt motivated after Mr.Ping interaction with the class.</t>
+  </si>
+  <si>
+    <t>Search is a good tool to navigate the  files efficiently. Also, find usages was effective.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motivated! </t>
+  </si>
+  <si>
+    <t>Select an open source project on GitHub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explored various open source projects available on GitHub, selected OpenRefine and submitted the pull request. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Narrowing down one project from a list of possible options was more difficult that expected. </t>
+  </si>
+  <si>
+    <t>A little unsure of the selected project.</t>
+  </si>
+  <si>
+    <t>10:00 pm - 10:30 pm</t>
+  </si>
+  <si>
+    <t>06:00 pm - 10:00 pm</t>
+  </si>
+  <si>
+    <t>11:00 am - 12:30 pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To complete the individual homework assigned. </t>
+  </si>
+  <si>
+    <t>Completed the given homework.</t>
+  </si>
+  <si>
+    <t>Figured out some details for adding the fruits to the game, though unsure of some details.</t>
+  </si>
+  <si>
+    <t>Hopefully what I submitted was correct.</t>
   </si>
 </sst>
 </file>
@@ -255,9 +330,6 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -275,6 +347,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -594,40 +669,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
-  <dimension ref="A1:G125"/>
+  <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.6640625" style="15" customWidth="1"/>
+    <col min="1" max="1" width="34.6640625" style="14" customWidth="1"/>
     <col min="2" max="7" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
     </row>
     <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="11"/>
+      <c r="A3" s="10"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -636,7 +711,7 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -649,10 +724,10 @@
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="1"/>
@@ -662,7 +737,7 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -675,7 +750,7 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
+      <c r="A7" s="10"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -684,7 +759,7 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -716,102 +791,172 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="13">
+      <c r="A10" s="12">
         <v>43839</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="D10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="F10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="G10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="8" t="s">
+    </row>
+    <row r="11" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="12">
+        <v>43843</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="12">
+        <v>43844</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="14"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="14"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="8"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="14"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="8"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="14"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="8"/>
+      <c r="C12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="78" x14ac:dyDescent="0.3">
+      <c r="A13" s="12">
+        <v>43846</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="12">
+        <v>43848</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="12">
+        <v>43849</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="14"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="8"/>
     </row>
     <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="7"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="6"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="8"/>
     </row>
     <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="14"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
-      <c r="D18" s="6"/>
+      <c r="D18" s="8"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="8"/>
     </row>
     <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="14"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="8"/>
@@ -820,7 +965,7 @@
       <c r="G19" s="8"/>
     </row>
     <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="14"/>
+      <c r="A20" s="13"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="8"/>
@@ -829,16 +974,16 @@
       <c r="G20" s="8"/>
     </row>
     <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="14"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
-      <c r="D21" s="8"/>
+      <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="8"/>
     </row>
     <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="14"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -847,7 +992,7 @@
       <c r="G22" s="8"/>
     </row>
     <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="14"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -856,7 +1001,7 @@
       <c r="G23" s="8"/>
     </row>
     <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="14"/>
+      <c r="A24" s="13"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -865,7 +1010,7 @@
       <c r="G24" s="8"/>
     </row>
     <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="14"/>
+      <c r="A25" s="13"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -874,7 +1019,7 @@
       <c r="G25" s="8"/>
     </row>
     <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="14"/>
+      <c r="A26" s="13"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -883,7 +1028,7 @@
       <c r="G26" s="8"/>
     </row>
     <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="14"/>
+      <c r="A27" s="13"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -892,7 +1037,7 @@
       <c r="G27" s="8"/>
     </row>
     <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="14"/>
+      <c r="A28" s="13"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -901,7 +1046,7 @@
       <c r="G28" s="8"/>
     </row>
     <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="14"/>
+      <c r="A29" s="13"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -910,7 +1055,7 @@
       <c r="G29" s="8"/>
     </row>
     <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="14"/>
+      <c r="A30" s="13"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -919,7 +1064,7 @@
       <c r="G30" s="8"/>
     </row>
     <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="14"/>
+      <c r="A31" s="13"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -928,7 +1073,7 @@
       <c r="G31" s="8"/>
     </row>
     <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="14"/>
+      <c r="A32" s="13"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -937,7 +1082,7 @@
       <c r="G32" s="8"/>
     </row>
     <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="14"/>
+      <c r="A33" s="13"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
@@ -946,7 +1091,7 @@
       <c r="G33" s="8"/>
     </row>
     <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="14"/>
+      <c r="A34" s="13"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
@@ -955,7 +1100,7 @@
       <c r="G34" s="8"/>
     </row>
     <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="14"/>
+      <c r="A35" s="13"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
@@ -964,7 +1109,7 @@
       <c r="G35" s="8"/>
     </row>
     <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="14"/>
+      <c r="A36" s="13"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -973,7 +1118,7 @@
       <c r="G36" s="8"/>
     </row>
     <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="14"/>
+      <c r="A37" s="13"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
@@ -982,7 +1127,7 @@
       <c r="G37" s="8"/>
     </row>
     <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="14"/>
+      <c r="A38" s="13"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
@@ -991,7 +1136,7 @@
       <c r="G38" s="8"/>
     </row>
     <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="14"/>
+      <c r="A39" s="13"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
@@ -1000,7 +1145,7 @@
       <c r="G39" s="8"/>
     </row>
     <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="14"/>
+      <c r="A40" s="13"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
@@ -1009,7 +1154,7 @@
       <c r="G40" s="8"/>
     </row>
     <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="14"/>
+      <c r="A41" s="13"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
@@ -1018,7 +1163,7 @@
       <c r="G41" s="8"/>
     </row>
     <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="14"/>
+      <c r="A42" s="13"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
@@ -1027,7 +1172,7 @@
       <c r="G42" s="8"/>
     </row>
     <row r="43" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="14"/>
+      <c r="A43" s="13"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
@@ -1036,7 +1181,7 @@
       <c r="G43" s="8"/>
     </row>
     <row r="44" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="14"/>
+      <c r="A44" s="13"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
@@ -1045,7 +1190,7 @@
       <c r="G44" s="8"/>
     </row>
     <row r="45" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="14"/>
+      <c r="A45" s="13"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
@@ -1054,7 +1199,7 @@
       <c r="G45" s="8"/>
     </row>
     <row r="46" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="14"/>
+      <c r="A46" s="13"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
@@ -1063,7 +1208,7 @@
       <c r="G46" s="8"/>
     </row>
     <row r="47" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="14"/>
+      <c r="A47" s="13"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
@@ -1072,7 +1217,7 @@
       <c r="G47" s="8"/>
     </row>
     <row r="48" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="14"/>
+      <c r="A48" s="13"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
@@ -1081,7 +1226,7 @@
       <c r="G48" s="8"/>
     </row>
     <row r="49" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="14"/>
+      <c r="A49" s="13"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
@@ -1090,7 +1235,7 @@
       <c r="G49" s="8"/>
     </row>
     <row r="50" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="14"/>
+      <c r="A50" s="13"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
@@ -1099,7 +1244,7 @@
       <c r="G50" s="8"/>
     </row>
     <row r="51" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="14"/>
+      <c r="A51" s="13"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
@@ -1108,7 +1253,7 @@
       <c r="G51" s="8"/>
     </row>
     <row r="52" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="14"/>
+      <c r="A52" s="13"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
@@ -1117,7 +1262,7 @@
       <c r="G52" s="8"/>
     </row>
     <row r="53" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="14"/>
+      <c r="A53" s="13"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
@@ -1126,7 +1271,7 @@
       <c r="G53" s="8"/>
     </row>
     <row r="54" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="14"/>
+      <c r="A54" s="13"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
@@ -1135,7 +1280,7 @@
       <c r="G54" s="8"/>
     </row>
     <row r="55" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="14"/>
+      <c r="A55" s="13"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
@@ -1144,7 +1289,7 @@
       <c r="G55" s="8"/>
     </row>
     <row r="56" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="14"/>
+      <c r="A56" s="13"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
@@ -1153,7 +1298,7 @@
       <c r="G56" s="8"/>
     </row>
     <row r="57" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A57" s="14"/>
+      <c r="A57" s="13"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
@@ -1162,7 +1307,7 @@
       <c r="G57" s="8"/>
     </row>
     <row r="58" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="14"/>
+      <c r="A58" s="13"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
@@ -1171,7 +1316,7 @@
       <c r="G58" s="8"/>
     </row>
     <row r="59" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="14"/>
+      <c r="A59" s="13"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
@@ -1180,7 +1325,7 @@
       <c r="G59" s="8"/>
     </row>
     <row r="60" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A60" s="14"/>
+      <c r="A60" s="13"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
@@ -1189,7 +1334,7 @@
       <c r="G60" s="8"/>
     </row>
     <row r="61" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="14"/>
+      <c r="A61" s="13"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
@@ -1198,7 +1343,7 @@
       <c r="G61" s="8"/>
     </row>
     <row r="62" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="14"/>
+      <c r="A62" s="13"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
@@ -1207,7 +1352,7 @@
       <c r="G62" s="8"/>
     </row>
     <row r="63" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A63" s="14"/>
+      <c r="A63" s="13"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
@@ -1216,7 +1361,7 @@
       <c r="G63" s="8"/>
     </row>
     <row r="64" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="14"/>
+      <c r="A64" s="13"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
@@ -1225,7 +1370,7 @@
       <c r="G64" s="8"/>
     </row>
     <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="14"/>
+      <c r="A65" s="13"/>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
@@ -1234,7 +1379,7 @@
       <c r="G65" s="8"/>
     </row>
     <row r="66" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="14"/>
+      <c r="A66" s="13"/>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
@@ -1243,7 +1388,7 @@
       <c r="G66" s="8"/>
     </row>
     <row r="67" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="14"/>
+      <c r="A67" s="13"/>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
@@ -1252,7 +1397,7 @@
       <c r="G67" s="8"/>
     </row>
     <row r="68" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A68" s="14"/>
+      <c r="A68" s="13"/>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
@@ -1261,7 +1406,7 @@
       <c r="G68" s="8"/>
     </row>
     <row r="69" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="14"/>
+      <c r="A69" s="13"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
@@ -1270,7 +1415,7 @@
       <c r="G69" s="8"/>
     </row>
     <row r="70" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A70" s="14"/>
+      <c r="A70" s="13"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
@@ -1279,7 +1424,7 @@
       <c r="G70" s="8"/>
     </row>
     <row r="71" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A71" s="14"/>
+      <c r="A71" s="13"/>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
@@ -1288,7 +1433,7 @@
       <c r="G71" s="8"/>
     </row>
     <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A72" s="14"/>
+      <c r="A72" s="13"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
@@ -1297,7 +1442,7 @@
       <c r="G72" s="8"/>
     </row>
     <row r="73" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A73" s="14"/>
+      <c r="A73" s="13"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
@@ -1306,7 +1451,7 @@
       <c r="G73" s="8"/>
     </row>
     <row r="74" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A74" s="14"/>
+      <c r="A74" s="13"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
       <c r="D74" s="7"/>
@@ -1315,7 +1460,7 @@
       <c r="G74" s="8"/>
     </row>
     <row r="75" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A75" s="14"/>
+      <c r="A75" s="13"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
@@ -1324,7 +1469,7 @@
       <c r="G75" s="8"/>
     </row>
     <row r="76" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="14"/>
+      <c r="A76" s="13"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
@@ -1333,7 +1478,7 @@
       <c r="G76" s="8"/>
     </row>
     <row r="77" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="14"/>
+      <c r="A77" s="13"/>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
@@ -1342,7 +1487,7 @@
       <c r="G77" s="8"/>
     </row>
     <row r="78" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A78" s="14"/>
+      <c r="A78" s="13"/>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
@@ -1351,7 +1496,7 @@
       <c r="G78" s="8"/>
     </row>
     <row r="79" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A79" s="14"/>
+      <c r="A79" s="13"/>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
@@ -1360,7 +1505,7 @@
       <c r="G79" s="8"/>
     </row>
     <row r="80" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A80" s="14"/>
+      <c r="A80" s="13"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
@@ -1369,7 +1514,7 @@
       <c r="G80" s="8"/>
     </row>
     <row r="81" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A81" s="14"/>
+      <c r="A81" s="13"/>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
@@ -1378,7 +1523,7 @@
       <c r="G81" s="8"/>
     </row>
     <row r="82" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A82" s="14"/>
+      <c r="A82" s="13"/>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
       <c r="D82" s="7"/>
@@ -1387,7 +1532,7 @@
       <c r="G82" s="8"/>
     </row>
     <row r="83" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A83" s="14"/>
+      <c r="A83" s="13"/>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
       <c r="D83" s="7"/>
@@ -1396,7 +1541,7 @@
       <c r="G83" s="8"/>
     </row>
     <row r="84" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A84" s="14"/>
+      <c r="A84" s="13"/>
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
       <c r="D84" s="7"/>
@@ -1405,7 +1550,7 @@
       <c r="G84" s="8"/>
     </row>
     <row r="85" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A85" s="14"/>
+      <c r="A85" s="13"/>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
@@ -1414,7 +1559,7 @@
       <c r="G85" s="8"/>
     </row>
     <row r="86" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A86" s="14"/>
+      <c r="A86" s="13"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
@@ -1423,7 +1568,7 @@
       <c r="G86" s="8"/>
     </row>
     <row r="87" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A87" s="14"/>
+      <c r="A87" s="13"/>
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
       <c r="D87" s="7"/>
@@ -1432,7 +1577,7 @@
       <c r="G87" s="8"/>
     </row>
     <row r="88" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A88" s="14"/>
+      <c r="A88" s="13"/>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
@@ -1441,7 +1586,7 @@
       <c r="G88" s="8"/>
     </row>
     <row r="89" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A89" s="14"/>
+      <c r="A89" s="13"/>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
       <c r="D89" s="7"/>
@@ -1450,7 +1595,7 @@
       <c r="G89" s="8"/>
     </row>
     <row r="90" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A90" s="14"/>
+      <c r="A90" s="13"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
@@ -1459,7 +1604,7 @@
       <c r="G90" s="8"/>
     </row>
     <row r="91" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A91" s="14"/>
+      <c r="A91" s="13"/>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
       <c r="D91" s="7"/>
@@ -1468,7 +1613,7 @@
       <c r="G91" s="8"/>
     </row>
     <row r="92" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A92" s="14"/>
+      <c r="A92" s="13"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
       <c r="D92" s="7"/>
@@ -1477,7 +1622,7 @@
       <c r="G92" s="8"/>
     </row>
     <row r="93" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A93" s="14"/>
+      <c r="A93" s="13"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
       <c r="D93" s="7"/>
@@ -1486,7 +1631,7 @@
       <c r="G93" s="8"/>
     </row>
     <row r="94" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A94" s="14"/>
+      <c r="A94" s="13"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
       <c r="D94" s="7"/>
@@ -1495,7 +1640,7 @@
       <c r="G94" s="8"/>
     </row>
     <row r="95" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A95" s="14"/>
+      <c r="A95" s="13"/>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
       <c r="D95" s="7"/>
@@ -1504,7 +1649,7 @@
       <c r="G95" s="8"/>
     </row>
     <row r="96" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A96" s="14"/>
+      <c r="A96" s="13"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
       <c r="D96" s="7"/>
@@ -1513,7 +1658,7 @@
       <c r="G96" s="8"/>
     </row>
     <row r="97" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A97" s="14"/>
+      <c r="A97" s="13"/>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
       <c r="D97" s="7"/>
@@ -1522,7 +1667,7 @@
       <c r="G97" s="8"/>
     </row>
     <row r="98" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A98" s="14"/>
+      <c r="A98" s="13"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
       <c r="D98" s="7"/>
@@ -1531,7 +1676,7 @@
       <c r="G98" s="8"/>
     </row>
     <row r="99" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A99" s="14"/>
+      <c r="A99" s="13"/>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
       <c r="D99" s="7"/>
@@ -1540,7 +1685,7 @@
       <c r="G99" s="8"/>
     </row>
     <row r="100" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A100" s="14"/>
+      <c r="A100" s="13"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
       <c r="D100" s="7"/>
@@ -1549,7 +1694,7 @@
       <c r="G100" s="8"/>
     </row>
     <row r="101" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A101" s="14"/>
+      <c r="A101" s="13"/>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
       <c r="D101" s="7"/>
@@ -1558,7 +1703,7 @@
       <c r="G101" s="8"/>
     </row>
     <row r="102" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A102" s="14"/>
+      <c r="A102" s="13"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
       <c r="D102" s="7"/>
@@ -1567,7 +1712,7 @@
       <c r="G102" s="8"/>
     </row>
     <row r="103" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A103" s="14"/>
+      <c r="A103" s="13"/>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
       <c r="D103" s="7"/>
@@ -1576,7 +1721,7 @@
       <c r="G103" s="8"/>
     </row>
     <row r="104" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A104" s="14"/>
+      <c r="A104" s="13"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
       <c r="D104" s="7"/>
@@ -1585,7 +1730,7 @@
       <c r="G104" s="8"/>
     </row>
     <row r="105" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A105" s="14"/>
+      <c r="A105" s="13"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
       <c r="D105" s="7"/>
@@ -1594,7 +1739,7 @@
       <c r="G105" s="8"/>
     </row>
     <row r="106" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A106" s="14"/>
+      <c r="A106" s="13"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
@@ -1603,7 +1748,7 @@
       <c r="G106" s="8"/>
     </row>
     <row r="107" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A107" s="14"/>
+      <c r="A107" s="13"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
       <c r="D107" s="7"/>
@@ -1612,7 +1757,7 @@
       <c r="G107" s="8"/>
     </row>
     <row r="108" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A108" s="14"/>
+      <c r="A108" s="13"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
       <c r="D108" s="7"/>
@@ -1621,7 +1766,7 @@
       <c r="G108" s="8"/>
     </row>
     <row r="109" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A109" s="14"/>
+      <c r="A109" s="13"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
       <c r="D109" s="7"/>
@@ -1630,7 +1775,7 @@
       <c r="G109" s="8"/>
     </row>
     <row r="110" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A110" s="14"/>
+      <c r="A110" s="13"/>
       <c r="B110" s="7"/>
       <c r="C110" s="7"/>
       <c r="D110" s="7"/>
@@ -1639,7 +1784,7 @@
       <c r="G110" s="8"/>
     </row>
     <row r="111" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A111" s="14"/>
+      <c r="A111" s="13"/>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
       <c r="D111" s="7"/>
@@ -1648,7 +1793,7 @@
       <c r="G111" s="8"/>
     </row>
     <row r="112" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A112" s="14"/>
+      <c r="A112" s="13"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
       <c r="D112" s="7"/>
@@ -1657,7 +1802,7 @@
       <c r="G112" s="8"/>
     </row>
     <row r="113" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A113" s="14"/>
+      <c r="A113" s="13"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
       <c r="D113" s="7"/>
@@ -1666,7 +1811,7 @@
       <c r="G113" s="8"/>
     </row>
     <row r="114" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A114" s="14"/>
+      <c r="A114" s="13"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
       <c r="D114" s="7"/>
@@ -1675,7 +1820,7 @@
       <c r="G114" s="8"/>
     </row>
     <row r="115" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A115" s="14"/>
+      <c r="A115" s="13"/>
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
       <c r="D115" s="7"/>
@@ -1684,7 +1829,7 @@
       <c r="G115" s="8"/>
     </row>
     <row r="116" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A116" s="14"/>
+      <c r="A116" s="13"/>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
       <c r="D116" s="7"/>
@@ -1693,7 +1838,7 @@
       <c r="G116" s="8"/>
     </row>
     <row r="117" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A117" s="14"/>
+      <c r="A117" s="13"/>
       <c r="B117" s="7"/>
       <c r="C117" s="7"/>
       <c r="D117" s="7"/>
@@ -1702,7 +1847,7 @@
       <c r="G117" s="8"/>
     </row>
     <row r="118" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A118" s="14"/>
+      <c r="A118" s="13"/>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
       <c r="D118" s="7"/>
@@ -1711,7 +1856,7 @@
       <c r="G118" s="8"/>
     </row>
     <row r="119" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A119" s="14"/>
+      <c r="A119" s="13"/>
       <c r="B119" s="7"/>
       <c r="C119" s="7"/>
       <c r="D119" s="7"/>
@@ -1720,7 +1865,7 @@
       <c r="G119" s="8"/>
     </row>
     <row r="120" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A120" s="14"/>
+      <c r="A120" s="13"/>
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
       <c r="D120" s="7"/>
@@ -1729,7 +1874,7 @@
       <c r="G120" s="8"/>
     </row>
     <row r="121" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A121" s="14"/>
+      <c r="A121" s="13"/>
       <c r="B121" s="7"/>
       <c r="C121" s="7"/>
       <c r="D121" s="7"/>
@@ -1738,7 +1883,7 @@
       <c r="G121" s="8"/>
     </row>
     <row r="122" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A122" s="14"/>
+      <c r="A122" s="13"/>
       <c r="B122" s="7"/>
       <c r="C122" s="7"/>
       <c r="D122" s="7"/>
@@ -1747,7 +1892,7 @@
       <c r="G122" s="8"/>
     </row>
     <row r="123" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A123" s="14"/>
+      <c r="A123" s="13"/>
       <c r="B123" s="7"/>
       <c r="C123" s="7"/>
       <c r="D123" s="7"/>
@@ -1756,22 +1901,13 @@
       <c r="G123" s="8"/>
     </row>
     <row r="124" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A124" s="14"/>
+      <c r="A124" s="13"/>
       <c r="B124" s="7"/>
       <c r="C124" s="7"/>
       <c r="D124" s="7"/>
       <c r="E124" s="7"/>
       <c r="F124" s="7"/>
       <c r="G124" s="8"/>
-    </row>
-    <row r="125" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A125" s="14"/>
-      <c r="B125" s="7"/>
-      <c r="C125" s="7"/>
-      <c r="D125" s="7"/>
-      <c r="E125" s="7"/>
-      <c r="F125" s="7"/>
-      <c r="G125" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Changes for Vaishakhi Pilankar Diary
</commit_message>
<xml_diff>
--- a/diaries/diary-vaishakhi-pilankar.xlsx
+++ b/diaries/diary-vaishakhi-pilankar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guds\Desktop\MSWE\CourseWork\Winter_2020\265P\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01BDA6D-95BA-47F5-BB5B-5878AF1968C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32C96C7-1C1D-40D6-A648-2385626F2F33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-108" windowWidth="22308" windowHeight="13176" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="68">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -166,13 +166,82 @@
   </si>
   <si>
     <t>Hopefully what I submitted was correct.</t>
+  </si>
+  <si>
+    <t>Learning new concepts</t>
+  </si>
+  <si>
+    <t>Understood the importance of having a visual model. Made a UML diagram for a project. Noted down the code flow while figuring out how a certain feature was implemented.</t>
+  </si>
+  <si>
+    <t>Having a mental model of a problem makes it easier for you to understand the flow of the code and hence helps you understand the code better.</t>
+  </si>
+  <si>
+    <t>Making UML diagram for a project is something that I didn’t know before. Excited to use it in the future.</t>
+  </si>
+  <si>
+    <t>Searching for a new open source project.</t>
+  </si>
+  <si>
+    <t>We were unsure of the previosuly selected project. Therefore we started searching for a new one. We decided on H2 database. We built the project and created a pull request for the same</t>
+  </si>
+  <si>
+    <t>We wanted to select elasticsearch but ended up not selecting it because it looked challenging. But we were not satisfied with the selected one. Then when we wanted to shift to elasticsearch again, we noticed that someone had already taken it. Realised we shouldnt have backed out on it just because it looked more challenging.</t>
+  </si>
+  <si>
+    <t>Happy that the new one got accepted.</t>
+  </si>
+  <si>
+    <t>12:00 pm - 03:00 pm</t>
+  </si>
+  <si>
+    <t>08:00 pm - 10:00 pm</t>
+  </si>
+  <si>
+    <t>Work on the homework given.</t>
+  </si>
+  <si>
+    <t>Created a UML diagram for the project. After taking a look decided on the create table and set user privilege features for the homework.</t>
+  </si>
+  <si>
+    <t>The UML for this project was pretty confusing. Navigating through the Uml was a task. Searching for a class in the UML almost seemed impossible.</t>
+  </si>
+  <si>
+    <t>Happy that we were atleast able to select two features.</t>
+  </si>
+  <si>
+    <t>10:00 pm - 01:00 am</t>
+  </si>
+  <si>
+    <t>Analysed the selected features and wrote down the flow in detail. We tried to make ourselves understand how the feature really worked and what it did. Finally able to figure out where in the UML diagram our classes were present.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Templates were helpful as we kept noting down many paths out of which only some were relevant. It made our analyzing easier. </t>
+  </si>
+  <si>
+    <t>Hopefully we have done enough.</t>
+  </si>
+  <si>
+    <t>10:00 am - 01:00 pm</t>
+  </si>
+  <si>
+    <t>Prepared the report.</t>
+  </si>
+  <si>
+    <t>Created a report to explain our findings. Created relevant UML classes diagrams.</t>
+  </si>
+  <si>
+    <t>Systematic approach taken by us helped us to create the report easily and efficienty.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wasn't an easy task. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,6 +333,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -304,7 +380,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -351,6 +427,10 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="18" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -669,16 +749,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
-  <dimension ref="A1:G124"/>
+  <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.6640625" style="14" customWidth="1"/>
-    <col min="2" max="7" width="34.6640625" customWidth="1"/>
+    <col min="2" max="3" width="34.6640625" customWidth="1"/>
+    <col min="4" max="4" width="34.6640625" style="17" customWidth="1"/>
+    <col min="5" max="7" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -701,7 +783,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -710,7 +792,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>1</v>
       </c>
@@ -723,7 +805,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
@@ -736,7 +818,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>3</v>
       </c>
@@ -749,7 +831,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -758,7 +840,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -767,7 +849,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -928,52 +1010,122 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="13"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="13"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="13"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="8"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="13"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="8"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="12">
+        <v>43850</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="156" x14ac:dyDescent="0.3">
+      <c r="A17" s="12">
+        <v>43856</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="78" x14ac:dyDescent="0.3">
+      <c r="A18" s="12">
+        <v>43856</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="12">
+        <v>43858</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="12">
+        <v>43860</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="13"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -982,7 +1134,7 @@
       <c r="F21" s="7"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="13"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -991,7 +1143,7 @@
       <c r="F22" s="7"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="13"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -1000,7 +1152,7 @@
       <c r="F23" s="7"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="13"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -1009,7 +1161,7 @@
       <c r="F24" s="7"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="13"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -1018,7 +1170,7 @@
       <c r="F25" s="7"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="13"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -1027,7 +1179,7 @@
       <c r="F26" s="7"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="13"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -1036,7 +1188,7 @@
       <c r="F27" s="7"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="13"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -1045,7 +1197,7 @@
       <c r="F28" s="7"/>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="13"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -1054,7 +1206,7 @@
       <c r="F29" s="7"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="13"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -1063,7 +1215,7 @@
       <c r="F30" s="7"/>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="13"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -1072,7 +1224,7 @@
       <c r="F31" s="7"/>
       <c r="G31" s="8"/>
     </row>
-    <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="13"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -1081,7 +1233,7 @@
       <c r="F32" s="7"/>
       <c r="G32" s="8"/>
     </row>
-    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="13"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -1090,7 +1242,7 @@
       <c r="F33" s="7"/>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="13"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -1099,7 +1251,7 @@
       <c r="F34" s="7"/>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="13"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -1108,7 +1260,7 @@
       <c r="F35" s="7"/>
       <c r="G35" s="8"/>
     </row>
-    <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="13"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -1117,7 +1269,7 @@
       <c r="F36" s="7"/>
       <c r="G36" s="8"/>
     </row>
-    <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="13"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -1126,7 +1278,7 @@
       <c r="F37" s="7"/>
       <c r="G37" s="8"/>
     </row>
-    <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="13"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -1135,7 +1287,7 @@
       <c r="F38" s="7"/>
       <c r="G38" s="8"/>
     </row>
-    <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="13"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -1144,7 +1296,7 @@
       <c r="F39" s="7"/>
       <c r="G39" s="8"/>
     </row>
-    <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="13"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -1153,7 +1305,7 @@
       <c r="F40" s="7"/>
       <c r="G40" s="8"/>
     </row>
-    <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="13"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -1162,7 +1314,7 @@
       <c r="F41" s="7"/>
       <c r="G41" s="8"/>
     </row>
-    <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="13"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -1171,7 +1323,7 @@
       <c r="F42" s="7"/>
       <c r="G42" s="8"/>
     </row>
-    <row r="43" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="13"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -1180,7 +1332,7 @@
       <c r="F43" s="7"/>
       <c r="G43" s="8"/>
     </row>
-    <row r="44" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="13"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -1189,7 +1341,7 @@
       <c r="F44" s="7"/>
       <c r="G44" s="8"/>
     </row>
-    <row r="45" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="13"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
@@ -1198,7 +1350,7 @@
       <c r="F45" s="7"/>
       <c r="G45" s="8"/>
     </row>
-    <row r="46" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="13"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -1207,7 +1359,7 @@
       <c r="F46" s="7"/>
       <c r="G46" s="8"/>
     </row>
-    <row r="47" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="13"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
@@ -1216,7 +1368,7 @@
       <c r="F47" s="7"/>
       <c r="G47" s="8"/>
     </row>
-    <row r="48" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="13"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -1225,7 +1377,7 @@
       <c r="F48" s="7"/>
       <c r="G48" s="8"/>
     </row>
-    <row r="49" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="13"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -1234,7 +1386,7 @@
       <c r="F49" s="7"/>
       <c r="G49" s="8"/>
     </row>
-    <row r="50" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="13"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
@@ -1243,7 +1395,7 @@
       <c r="F50" s="7"/>
       <c r="G50" s="8"/>
     </row>
-    <row r="51" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="13"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
@@ -1252,7 +1404,7 @@
       <c r="F51" s="7"/>
       <c r="G51" s="8"/>
     </row>
-    <row r="52" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="13"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
@@ -1261,7 +1413,7 @@
       <c r="F52" s="7"/>
       <c r="G52" s="8"/>
     </row>
-    <row r="53" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="13"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -1270,7 +1422,7 @@
       <c r="F53" s="7"/>
       <c r="G53" s="8"/>
     </row>
-    <row r="54" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="13"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
@@ -1279,7 +1431,7 @@
       <c r="F54" s="7"/>
       <c r="G54" s="8"/>
     </row>
-    <row r="55" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="13"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -1288,7 +1440,7 @@
       <c r="F55" s="7"/>
       <c r="G55" s="8"/>
     </row>
-    <row r="56" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="13"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
@@ -1297,7 +1449,7 @@
       <c r="F56" s="7"/>
       <c r="G56" s="8"/>
     </row>
-    <row r="57" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="13"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
@@ -1306,7 +1458,7 @@
       <c r="F57" s="7"/>
       <c r="G57" s="8"/>
     </row>
-    <row r="58" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="13"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
@@ -1315,7 +1467,7 @@
       <c r="F58" s="7"/>
       <c r="G58" s="8"/>
     </row>
-    <row r="59" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="13"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
@@ -1324,7 +1476,7 @@
       <c r="F59" s="7"/>
       <c r="G59" s="8"/>
     </row>
-    <row r="60" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="13"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
@@ -1333,7 +1485,7 @@
       <c r="F60" s="7"/>
       <c r="G60" s="8"/>
     </row>
-    <row r="61" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="13"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
@@ -1342,7 +1494,7 @@
       <c r="F61" s="7"/>
       <c r="G61" s="8"/>
     </row>
-    <row r="62" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="13"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
@@ -1351,7 +1503,7 @@
       <c r="F62" s="7"/>
       <c r="G62" s="8"/>
     </row>
-    <row r="63" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="13"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
@@ -1360,7 +1512,7 @@
       <c r="F63" s="7"/>
       <c r="G63" s="8"/>
     </row>
-    <row r="64" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="13"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
@@ -1369,7 +1521,7 @@
       <c r="F64" s="7"/>
       <c r="G64" s="8"/>
     </row>
-    <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="13"/>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
@@ -1378,7 +1530,7 @@
       <c r="F65" s="7"/>
       <c r="G65" s="8"/>
     </row>
-    <row r="66" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="13"/>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
@@ -1387,7 +1539,7 @@
       <c r="F66" s="7"/>
       <c r="G66" s="8"/>
     </row>
-    <row r="67" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="13"/>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
@@ -1396,7 +1548,7 @@
       <c r="F67" s="7"/>
       <c r="G67" s="8"/>
     </row>
-    <row r="68" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="13"/>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
@@ -1405,7 +1557,7 @@
       <c r="F68" s="7"/>
       <c r="G68" s="8"/>
     </row>
-    <row r="69" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="13"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
@@ -1414,7 +1566,7 @@
       <c r="F69" s="7"/>
       <c r="G69" s="8"/>
     </row>
-    <row r="70" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="13"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
@@ -1423,7 +1575,7 @@
       <c r="F70" s="7"/>
       <c r="G70" s="8"/>
     </row>
-    <row r="71" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="13"/>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
@@ -1432,7 +1584,7 @@
       <c r="F71" s="7"/>
       <c r="G71" s="8"/>
     </row>
-    <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="13"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
@@ -1441,7 +1593,7 @@
       <c r="F72" s="7"/>
       <c r="G72" s="8"/>
     </row>
-    <row r="73" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="13"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
@@ -1450,7 +1602,7 @@
       <c r="F73" s="7"/>
       <c r="G73" s="8"/>
     </row>
-    <row r="74" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="13"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
@@ -1459,7 +1611,7 @@
       <c r="F74" s="7"/>
       <c r="G74" s="8"/>
     </row>
-    <row r="75" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="13"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
@@ -1468,7 +1620,7 @@
       <c r="F75" s="7"/>
       <c r="G75" s="8"/>
     </row>
-    <row r="76" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="13"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
@@ -1477,7 +1629,7 @@
       <c r="F76" s="7"/>
       <c r="G76" s="8"/>
     </row>
-    <row r="77" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="13"/>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
@@ -1486,7 +1638,7 @@
       <c r="F77" s="7"/>
       <c r="G77" s="8"/>
     </row>
-    <row r="78" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="13"/>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
@@ -1495,7 +1647,7 @@
       <c r="F78" s="7"/>
       <c r="G78" s="8"/>
     </row>
-    <row r="79" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="13"/>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
@@ -1504,7 +1656,7 @@
       <c r="F79" s="7"/>
       <c r="G79" s="8"/>
     </row>
-    <row r="80" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="13"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
@@ -1513,7 +1665,7 @@
       <c r="F80" s="7"/>
       <c r="G80" s="8"/>
     </row>
-    <row r="81" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="13"/>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
@@ -1522,7 +1674,7 @@
       <c r="F81" s="7"/>
       <c r="G81" s="8"/>
     </row>
-    <row r="82" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="13"/>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
@@ -1531,7 +1683,7 @@
       <c r="F82" s="7"/>
       <c r="G82" s="8"/>
     </row>
-    <row r="83" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="13"/>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
@@ -1540,7 +1692,7 @@
       <c r="F83" s="7"/>
       <c r="G83" s="8"/>
     </row>
-    <row r="84" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="13"/>
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
@@ -1549,7 +1701,7 @@
       <c r="F84" s="7"/>
       <c r="G84" s="8"/>
     </row>
-    <row r="85" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="13"/>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
@@ -1558,7 +1710,7 @@
       <c r="F85" s="7"/>
       <c r="G85" s="8"/>
     </row>
-    <row r="86" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="13"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
@@ -1567,7 +1719,7 @@
       <c r="F86" s="7"/>
       <c r="G86" s="8"/>
     </row>
-    <row r="87" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="13"/>
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
@@ -1576,7 +1728,7 @@
       <c r="F87" s="7"/>
       <c r="G87" s="8"/>
     </row>
-    <row r="88" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="13"/>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
@@ -1585,7 +1737,7 @@
       <c r="F88" s="7"/>
       <c r="G88" s="8"/>
     </row>
-    <row r="89" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="13"/>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
@@ -1594,7 +1746,7 @@
       <c r="F89" s="7"/>
       <c r="G89" s="8"/>
     </row>
-    <row r="90" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="13"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
@@ -1603,7 +1755,7 @@
       <c r="F90" s="7"/>
       <c r="G90" s="8"/>
     </row>
-    <row r="91" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="13"/>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
@@ -1612,7 +1764,7 @@
       <c r="F91" s="7"/>
       <c r="G91" s="8"/>
     </row>
-    <row r="92" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="13"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
@@ -1621,7 +1773,7 @@
       <c r="F92" s="7"/>
       <c r="G92" s="8"/>
     </row>
-    <row r="93" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="13"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
@@ -1630,7 +1782,7 @@
       <c r="F93" s="7"/>
       <c r="G93" s="8"/>
     </row>
-    <row r="94" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="13"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
@@ -1639,7 +1791,7 @@
       <c r="F94" s="7"/>
       <c r="G94" s="8"/>
     </row>
-    <row r="95" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="13"/>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
@@ -1648,7 +1800,7 @@
       <c r="F95" s="7"/>
       <c r="G95" s="8"/>
     </row>
-    <row r="96" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="13"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
@@ -1657,7 +1809,7 @@
       <c r="F96" s="7"/>
       <c r="G96" s="8"/>
     </row>
-    <row r="97" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="13"/>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
@@ -1666,7 +1818,7 @@
       <c r="F97" s="7"/>
       <c r="G97" s="8"/>
     </row>
-    <row r="98" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="13"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
@@ -1675,7 +1827,7 @@
       <c r="F98" s="7"/>
       <c r="G98" s="8"/>
     </row>
-    <row r="99" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="13"/>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
@@ -1684,7 +1836,7 @@
       <c r="F99" s="7"/>
       <c r="G99" s="8"/>
     </row>
-    <row r="100" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="13"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
@@ -1693,7 +1845,7 @@
       <c r="F100" s="7"/>
       <c r="G100" s="8"/>
     </row>
-    <row r="101" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="13"/>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
@@ -1702,7 +1854,7 @@
       <c r="F101" s="7"/>
       <c r="G101" s="8"/>
     </row>
-    <row r="102" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="13"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
@@ -1711,7 +1863,7 @@
       <c r="F102" s="7"/>
       <c r="G102" s="8"/>
     </row>
-    <row r="103" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="13"/>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
@@ -1720,7 +1872,7 @@
       <c r="F103" s="7"/>
       <c r="G103" s="8"/>
     </row>
-    <row r="104" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="13"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
@@ -1729,7 +1881,7 @@
       <c r="F104" s="7"/>
       <c r="G104" s="8"/>
     </row>
-    <row r="105" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="13"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
@@ -1738,7 +1890,7 @@
       <c r="F105" s="7"/>
       <c r="G105" s="8"/>
     </row>
-    <row r="106" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="13"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
@@ -1747,7 +1899,7 @@
       <c r="F106" s="7"/>
       <c r="G106" s="8"/>
     </row>
-    <row r="107" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="13"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
@@ -1756,7 +1908,7 @@
       <c r="F107" s="7"/>
       <c r="G107" s="8"/>
     </row>
-    <row r="108" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="13"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
@@ -1765,7 +1917,7 @@
       <c r="F108" s="7"/>
       <c r="G108" s="8"/>
     </row>
-    <row r="109" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="13"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
@@ -1774,7 +1926,7 @@
       <c r="F109" s="7"/>
       <c r="G109" s="8"/>
     </row>
-    <row r="110" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="13"/>
       <c r="B110" s="7"/>
       <c r="C110" s="7"/>
@@ -1783,7 +1935,7 @@
       <c r="F110" s="7"/>
       <c r="G110" s="8"/>
     </row>
-    <row r="111" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="13"/>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
@@ -1792,7 +1944,7 @@
       <c r="F111" s="7"/>
       <c r="G111" s="8"/>
     </row>
-    <row r="112" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="13"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
@@ -1801,7 +1953,7 @@
       <c r="F112" s="7"/>
       <c r="G112" s="8"/>
     </row>
-    <row r="113" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="13"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
@@ -1810,7 +1962,7 @@
       <c r="F113" s="7"/>
       <c r="G113" s="8"/>
     </row>
-    <row r="114" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="13"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
@@ -1819,7 +1971,7 @@
       <c r="F114" s="7"/>
       <c r="G114" s="8"/>
     </row>
-    <row r="115" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="13"/>
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
@@ -1828,7 +1980,7 @@
       <c r="F115" s="7"/>
       <c r="G115" s="8"/>
     </row>
-    <row r="116" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" s="13"/>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
@@ -1837,7 +1989,7 @@
       <c r="F116" s="7"/>
       <c r="G116" s="8"/>
     </row>
-    <row r="117" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" s="13"/>
       <c r="B117" s="7"/>
       <c r="C117" s="7"/>
@@ -1846,7 +1998,7 @@
       <c r="F117" s="7"/>
       <c r="G117" s="8"/>
     </row>
-    <row r="118" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" s="13"/>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
@@ -1855,7 +2007,7 @@
       <c r="F118" s="7"/>
       <c r="G118" s="8"/>
     </row>
-    <row r="119" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" s="13"/>
       <c r="B119" s="7"/>
       <c r="C119" s="7"/>
@@ -1864,7 +2016,7 @@
       <c r="F119" s="7"/>
       <c r="G119" s="8"/>
     </row>
-    <row r="120" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" s="13"/>
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
@@ -1873,7 +2025,7 @@
       <c r="F120" s="7"/>
       <c r="G120" s="8"/>
     </row>
-    <row r="121" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="13"/>
       <c r="B121" s="7"/>
       <c r="C121" s="7"/>
@@ -1882,7 +2034,7 @@
       <c r="F121" s="7"/>
       <c r="G121" s="8"/>
     </row>
-    <row r="122" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="13"/>
       <c r="B122" s="7"/>
       <c r="C122" s="7"/>
@@ -1891,7 +2043,7 @@
       <c r="F122" s="7"/>
       <c r="G122" s="8"/>
     </row>
-    <row r="123" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" s="13"/>
       <c r="B123" s="7"/>
       <c r="C123" s="7"/>
@@ -1899,15 +2051,6 @@
       <c r="E123" s="7"/>
       <c r="F123" s="7"/>
       <c r="G123" s="8"/>
-    </row>
-    <row r="124" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A124" s="13"/>
-      <c r="B124" s="7"/>
-      <c r="C124" s="7"/>
-      <c r="D124" s="7"/>
-      <c r="E124" s="7"/>
-      <c r="F124" s="7"/>
-      <c r="G124" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Changes to diary committed
</commit_message>
<xml_diff>
--- a/diaries/diary-vaishakhi-pilankar.xlsx
+++ b/diaries/diary-vaishakhi-pilankar.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guds\Desktop\MSWE\CourseWork\Winter_2020\265P\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32C96C7-1C1D-40D6-A648-2385626F2F33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCB279A-9C7B-42B8-9428-E285C5EB197C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-108" windowWidth="22308" windowHeight="13176" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="93">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -235,6 +235,81 @@
   </si>
   <si>
     <t xml:space="preserve">Wasn't an easy task. </t>
+  </si>
+  <si>
+    <t>08:00 pm - 09:00 pm</t>
+  </si>
+  <si>
+    <t>To understand what was taught in the previous class.</t>
+  </si>
+  <si>
+    <t>Anjana and Aman explained about the key practises in reverse engineering and many ways to model the architecture.</t>
+  </si>
+  <si>
+    <t>We need to properly understand the code, because if we don’t it might lead to wrong assumptions and might affect out future decisions on it.</t>
+  </si>
+  <si>
+    <t>Excited to do the upcoming homework with this understanding.</t>
+  </si>
+  <si>
+    <t>To decide which features we would work on for the next homework.And how data is actually stored from h2 onto the disk.</t>
+  </si>
+  <si>
+    <t>We figured out the first feature. Second feature was work in progress and we decided to continue it the next time.</t>
+  </si>
+  <si>
+    <t>We had some problems running the application. The .jar file was not gettign detected so we had to downgrade our java version and edit the system path in pom.xml and do a clean project. Finding usages is a great help to discover the code flow.</t>
+  </si>
+  <si>
+    <t>Happy we could get the application running.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We were not completely satisfied with our second feature so we decided to choose a new one to see how insert/delete works. </t>
+  </si>
+  <si>
+    <t>Able to somewhat figure out the next feature.</t>
+  </si>
+  <si>
+    <t>It was really hard figuring out the former feature.</t>
+  </si>
+  <si>
+    <t>Little frustated about not understanding the previous feature.</t>
+  </si>
+  <si>
+    <t>10:00 am - 12:00 pm</t>
+  </si>
+  <si>
+    <t>Complete figuring out the second figure.</t>
+  </si>
+  <si>
+    <t>11:00 am - 01:00 pm                    09:30 pm - 11:00 pm</t>
+  </si>
+  <si>
+    <t>We were able to figure out how this new feature works and able to draw out diagrams.</t>
+  </si>
+  <si>
+    <t>It was a little difficult to understand the code as we went a little deep into it as there were many attributes and functions that we had to make ourselves familiar with.</t>
+  </si>
+  <si>
+    <t>Happy that we could understand the feature.</t>
+  </si>
+  <si>
+    <t>10:00 pm - 02:00 am</t>
+  </si>
+  <si>
+    <t>10:00 am - 12:30 pm</t>
+  </si>
+  <si>
+    <t>Finishing the report</t>
+  </si>
+  <si>
+    <t>We finished writing our report complete with all the diagrams.</t>
+  </si>
+  <si>
+    <t>Because we had everything understood properly, we could easily write a report.</t>
+  </si>
+  <si>
+    <t>Happy to be able to complete everything in time.</t>
   </si>
 </sst>
 </file>
@@ -424,13 +499,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="18" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -751,37 +826,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.6640625" style="14" customWidth="1"/>
     <col min="2" max="3" width="34.6640625" customWidth="1"/>
-    <col min="4" max="4" width="34.6640625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="34.6640625" style="16" customWidth="1"/>
     <col min="5" max="7" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
@@ -1060,7 +1135,7 @@
       <c r="A18" s="12">
         <v>43856</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="15" t="s">
         <v>54</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1125,50 +1200,120 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="13"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="8"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="13"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="8"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="13"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="8"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="13"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="8"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="13"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="8"/>
+    <row r="21" spans="1:7" ht="78" x14ac:dyDescent="0.3">
+      <c r="A21" s="12">
+        <v>43861</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="12">
+        <v>43864</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="12">
+        <v>43865</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="12">
+        <v>43866</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="12">
+        <v>43867</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="13"/>

</xml_diff>

<commit_message>
Vaishakhi Pilankar 06 Feb Diary
</commit_message>
<xml_diff>
--- a/diaries/diary-vaishakhi-pilankar.xlsx
+++ b/diaries/diary-vaishakhi-pilankar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guds\Desktop\MSWE\CourseWork\Winter_2020\265P\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCB279A-9C7B-42B8-9428-E285C5EB197C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF4D490-A93B-41EF-AE10-75884FC2086F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-108" windowWidth="22308" windowHeight="13176" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="96">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -310,6 +310,15 @@
   </si>
   <si>
     <t>Happy to be able to complete everything in time.</t>
+  </si>
+  <si>
+    <t>We learned about the key expert practices.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Realised how the KEP helped while trying to understand a slightly difficult code which had no documentation. </t>
+  </si>
+  <si>
+    <t>Nervous for midterm, Don’t know what to expect.</t>
   </si>
 </sst>
 </file>
@@ -826,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="C23" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1315,14 +1324,28 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="13"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="8"/>
+    <row r="26" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A26" s="12">
+        <v>43867</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="13"/>

</xml_diff>

<commit_message>
Added diary for last week
</commit_message>
<xml_diff>
--- a/diaries/diary-vaishakhi-pilankar.xlsx
+++ b/diaries/diary-vaishakhi-pilankar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guds\Desktop\MSWE\CourseWork\Winter_2020\265P\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF4D490-A93B-41EF-AE10-75884FC2086F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DE0EAE-9941-40A3-9A44-9D9419A0549D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-108" windowWidth="22308" windowHeight="13176" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="114">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -319,6 +319,60 @@
   </si>
   <si>
     <t>Nervous for midterm, Don’t know what to expect.</t>
+  </si>
+  <si>
+    <t>09:00 am - 12:00 pm</t>
+  </si>
+  <si>
+    <t>Complete revision for the test</t>
+  </si>
+  <si>
+    <t>Referred to the slides and some articles on the internet to get a better understanding of the concepts like all the different types of structural and behavioral diagrams.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since I had paid attention in class, it was easier to revise, as after reiterating the examples given in class to explain the concepts my understanding of it had greatly increased. </t>
+  </si>
+  <si>
+    <t>I feel like Ive prepared enough. But still nervous as this is my first exam in 3 years!</t>
+  </si>
+  <si>
+    <t>Successfully complete the test and learn something new!</t>
+  </si>
+  <si>
+    <t>I feel like I wasted my time on answers when it could've been completed in less time and that’s why I had to rush a little in the end and couldn't really write down all the points I wanted to for the last question. But overall good paper</t>
+  </si>
+  <si>
+    <t>Test went well! Also learned other points of KEP and the big picture like the stakeholders, the developers etc.</t>
+  </si>
+  <si>
+    <t>Next time I will manage my time better while giving an exam.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gained a better understanding of how explanation of the flow must be done. Like giving more diagrams so the reader can relate to the given explanation of it better. </t>
+  </si>
+  <si>
+    <t>Hopefully our score for the frist assignment would increase.</t>
+  </si>
+  <si>
+    <t>To resubmit our first homework and start with the next homework</t>
+  </si>
+  <si>
+    <t>We added the missing UML diagrams and also explained the flow more clearly this time.Explained the features of the application.</t>
+  </si>
+  <si>
+    <t>11:00 pm - 12:00 am</t>
+  </si>
+  <si>
+    <t>To complete our assigment 3.</t>
+  </si>
+  <si>
+    <t>We completed our assignment 3 and put as much as relevant information needed. Formatted the document so that it would be pleasing to the reader.Succesfully selected the open issues which we think we can tackle. Also managed to find stakeholders of the application.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It had many stakeholders to begin with. Realised why our application is unique. </t>
+  </si>
+  <si>
+    <t>Hopefully we have done a better job and that we don’t have to resubmit this assigment too.</t>
   </si>
 </sst>
 </file>
@@ -835,8 +889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C23" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="C29" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1347,41 +1401,97 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="13"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="8"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="13"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="8"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="13"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="8"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="13"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="8"/>
+    <row r="27" spans="1:7" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="12">
+        <v>43874</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="12">
+        <v>43874</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="78" x14ac:dyDescent="0.3">
+      <c r="A29" s="12">
+        <v>43876</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="140.4" x14ac:dyDescent="0.3">
+      <c r="A30" s="12">
+        <v>43880</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="13"/>

</xml_diff>

<commit_message>
Revert "Added diary for last week"
This reverts commit 47ae6283f269992d1f5df2f1c0227812a04438f9.

Revert to original
</commit_message>
<xml_diff>
--- a/diaries/diary-vaishakhi-pilankar.xlsx
+++ b/diaries/diary-vaishakhi-pilankar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guds\Desktop\MSWE\CourseWork\Winter_2020\265P\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DE0EAE-9941-40A3-9A44-9D9419A0549D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF4D490-A93B-41EF-AE10-75884FC2086F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-108" windowWidth="22308" windowHeight="13176" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="96">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -319,60 +319,6 @@
   </si>
   <si>
     <t>Nervous for midterm, Don’t know what to expect.</t>
-  </si>
-  <si>
-    <t>09:00 am - 12:00 pm</t>
-  </si>
-  <si>
-    <t>Complete revision for the test</t>
-  </si>
-  <si>
-    <t>Referred to the slides and some articles on the internet to get a better understanding of the concepts like all the different types of structural and behavioral diagrams.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Since I had paid attention in class, it was easier to revise, as after reiterating the examples given in class to explain the concepts my understanding of it had greatly increased. </t>
-  </si>
-  <si>
-    <t>I feel like Ive prepared enough. But still nervous as this is my first exam in 3 years!</t>
-  </si>
-  <si>
-    <t>Successfully complete the test and learn something new!</t>
-  </si>
-  <si>
-    <t>I feel like I wasted my time on answers when it could've been completed in less time and that’s why I had to rush a little in the end and couldn't really write down all the points I wanted to for the last question. But overall good paper</t>
-  </si>
-  <si>
-    <t>Test went well! Also learned other points of KEP and the big picture like the stakeholders, the developers etc.</t>
-  </si>
-  <si>
-    <t>Next time I will manage my time better while giving an exam.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gained a better understanding of how explanation of the flow must be done. Like giving more diagrams so the reader can relate to the given explanation of it better. </t>
-  </si>
-  <si>
-    <t>Hopefully our score for the frist assignment would increase.</t>
-  </si>
-  <si>
-    <t>To resubmit our first homework and start with the next homework</t>
-  </si>
-  <si>
-    <t>We added the missing UML diagrams and also explained the flow more clearly this time.Explained the features of the application.</t>
-  </si>
-  <si>
-    <t>11:00 pm - 12:00 am</t>
-  </si>
-  <si>
-    <t>To complete our assigment 3.</t>
-  </si>
-  <si>
-    <t>We completed our assignment 3 and put as much as relevant information needed. Formatted the document so that it would be pleasing to the reader.Succesfully selected the open issues which we think we can tackle. Also managed to find stakeholders of the application.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It had many stakeholders to begin with. Realised why our application is unique. </t>
-  </si>
-  <si>
-    <t>Hopefully we have done a better job and that we don’t have to resubmit this assigment too.</t>
   </si>
 </sst>
 </file>
@@ -889,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C29" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="C23" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1401,97 +1347,41 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="12">
-        <v>43874</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="12">
-        <v>43874</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="78" x14ac:dyDescent="0.3">
-      <c r="A29" s="12">
-        <v>43876</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="140.4" x14ac:dyDescent="0.3">
-      <c r="A30" s="12">
-        <v>43880</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>113</v>
-      </c>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="13"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="8"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="13"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="8"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="13"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="8"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="13"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="8"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="13"/>

</xml_diff>